<commit_message>
write to productcastinglist db OK
</commit_message>
<xml_diff>
--- a/data/globalTables/finalPacking.xlsx
+++ b/data/globalTables/finalPacking.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Tools\TCPIP communication\zihua_MESSystem\data\globalTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\MESSystem_180506\MESSystem\data\globalTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="45" windowWidth="14355" windowHeight="5580"/>
+    <workbookView xWindow="1290" yWindow="45" windowWidth="14355" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t>productCode</t>
   </si>
@@ -128,6 +128,10 @@
   </si>
   <si>
     <t>barcode</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>machineID</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -509,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -558,8 +562,8 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A2">
-        <v>19</v>
+      <c r="A2" t="s">
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>27</v>

</xml_diff>